<commit_message>
make summary stats table
</commit_message>
<xml_diff>
--- a/output/1-never-married.xlsx
+++ b/output/1-never-married.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tianl\Documents\GitHub\parental-wealth-impact\output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ltian\OneDrive - homesite.com\Documents\workspace\github_workspace\parental-wealth-impact\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AE46317-2CAD-45FA-AB05-5FC2B3ABF2E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="5_{01AC26B7-F215-41C2-B818-83102B1A4774}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet 1" sheetId="1" r:id="rId1"/>
@@ -133,7 +133,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -156,7 +156,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -256,18 +256,18 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -567,31 +567,31 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="39.08984375" customWidth="1"/>
-    <col min="2" max="3" width="12.81640625" customWidth="1"/>
+    <col min="1" max="1" width="39.109375" customWidth="1"/>
+    <col min="2" max="3" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="10" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -602,14 +602,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3">
       <c r="A4" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
         <v>24</v>
       </c>
@@ -620,7 +620,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
         <v>25</v>
       </c>
@@ -631,7 +631,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
         <v>26</v>
       </c>
@@ -642,7 +642,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
         <v>27</v>
       </c>
@@ -653,14 +653,14 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3">
       <c r="A9" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3">
       <c r="A10" s="2" t="s">
         <v>29</v>
       </c>
@@ -671,7 +671,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3">
       <c r="A11" s="2" t="s">
         <v>30</v>
       </c>
@@ -682,7 +682,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
         <v>31</v>
       </c>
@@ -693,7 +693,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3">
       <c r="A13" s="5" t="s">
         <v>2</v>
       </c>
@@ -704,7 +704,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3">
       <c r="A14" s="5" t="s">
         <v>3</v>
       </c>
@@ -715,7 +715,7 @@
         <v>211.08</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3">
       <c r="A15" s="5" t="s">
         <v>4</v>
       </c>
@@ -726,7 +726,7 @@
         <v>248.32</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3">
       <c r="A16" s="6" t="s">
         <v>5</v>
       </c>
@@ -737,14 +737,14 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="11" t="s">
+    <row r="17" spans="1:3">
+      <c r="A17" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="12" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>